<commit_message>
Avance generación de constancia de pago.
</commit_message>
<xml_diff>
--- a/docs/formatos-carga/editar - webservice.xlsx
+++ b/docs/formatos-carga/editar - webservice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\repos\00043-DWeb-CuentasPorCobrar\docs\formatos-carga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9FCB9D-8F0D-4791-A591-98DC762838D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D40FD0-B88A-4B0D-877B-31E2531E147B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{AA7C1ECB-C44D-4F0F-9EED-46EBFA85A98E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA7C1ECB-C44D-4F0F-9EED-46EBFA85A98E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -136,8 +136,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,14 +455,14 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -471,20 +471,20 @@
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
@@ -511,7 +511,7 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -519,13 +519,13 @@
       <c r="A2">
         <v>24512</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>2022032732</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>9479865</v>
       </c>
       <c r="E2" t="s">

</xml_diff>